<commit_message>
COmmit Verified : Updated Logic, changed photos
</commit_message>
<xml_diff>
--- a/sheet.xlsx
+++ b/sheet.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,20 +458,40 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>21331a0560</t>
+          <t>21331a0562</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>Q1</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Q7</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>21331a0569</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>Q4</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Q17</t>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Q10</t>
         </is>
       </c>
     </row>

</xml_diff>